<commit_message>
feat: Changed audio sample and added in real names of individuals involved
</commit_message>
<xml_diff>
--- a/audio_samples/Bodycam URLs.xlsx
+++ b/audio_samples/Bodycam URLs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\Github Projects\Police Audio Assistance Client\Audio Samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\Github Projects\ElevenLabs Hackathon\audio_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FA330F-5FC2-45E0-B128-6C44CDCD838B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A93DCD-347C-47CC-B89F-64FEF882D75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -386,7 +386,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C36" sqref="C35:C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>